<commit_message>
Added Edit User, Adjustments (Tanggal, Jenis & Nilai Risiko).
</commit_message>
<xml_diff>
--- a/Format Excel Empty.xlsx
+++ b/Format Excel Empty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\manajemenrisiko\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEC9ADD-8DC5-442E-8147-075F47B19A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C412E9-1D16-4411-942C-2ECAB73B053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A0ADA62E-DC35-4BDA-9025-A7A47BBECDD3}"/>
   </bookViews>
@@ -120,7 +120,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-_);_(@_)"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,11 +159,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="20"/>
       <name val="Calibri"/>
@@ -491,7 +486,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -520,21 +515,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -546,18 +532,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -572,27 +546,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -600,36 +559,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -644,6 +573,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -654,6 +589,45 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -972,13 +946,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6BE6975-4408-432E-86E2-0469528F907B}">
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" customWidth="1"/>
     <col min="2" max="2" width="21.88671875" customWidth="1"/>
@@ -997,232 +971,232 @@
     <col min="23" max="23" width="26.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="16.2" customHeight="1" thickBot="1">
-      <c r="B1" s="31"/>
-    </row>
-    <row r="2" spans="1:23" ht="17.399999999999999" customHeight="1" thickBot="1">
-      <c r="A2" s="26" t="s">
+    <row r="1" spans="1:23" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="24"/>
+    </row>
+    <row r="2" spans="1:23" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="42" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="44"/>
-    </row>
-    <row r="3" spans="1:23" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A3" s="28" t="s">
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="45"/>
+      <c r="W2" s="46"/>
+    </row>
+    <row r="3" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
-      <c r="W3" s="47"/>
-    </row>
-    <row r="4" spans="1:23" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A4" s="28" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="49"/>
+    </row>
+    <row r="4" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
-      <c r="R4" s="46"/>
-      <c r="S4" s="46"/>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46"/>
-      <c r="V4" s="46"/>
-      <c r="W4" s="47"/>
-    </row>
-    <row r="5" spans="1:23" ht="16.8" thickTop="1" thickBot="1">
-      <c r="A5" s="28" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="49"/>
+    </row>
+    <row r="5" spans="1:23" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="W5" s="47"/>
-    </row>
-    <row r="6" spans="1:23" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A6" s="29"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="49"/>
-      <c r="R6" s="49"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="49"/>
-      <c r="U6" s="49"/>
-      <c r="V6" s="49"/>
-      <c r="W6" s="50"/>
-    </row>
-    <row r="7" spans="1:23" ht="27.6" customHeight="1" thickBot="1">
-      <c r="A7" s="51" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="49"/>
+    </row>
+    <row r="6" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="51"/>
+      <c r="R6" s="51"/>
+      <c r="S6" s="51"/>
+      <c r="T6" s="51"/>
+      <c r="U6" s="51"/>
+      <c r="V6" s="51"/>
+      <c r="W6" s="52"/>
+    </row>
+    <row r="7" spans="1:23" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="56" t="s">
+      <c r="E7" s="35"/>
+      <c r="F7" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="57"/>
-      <c r="H7" s="39" t="s">
+      <c r="G7" s="37"/>
+      <c r="H7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="51" t="s">
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="39" t="s">
+      <c r="O7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="40"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="41"/>
-      <c r="U7" s="36" t="s">
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="V7" s="37"/>
-      <c r="W7" s="38"/>
-    </row>
-    <row r="8" spans="1:23" ht="27.6" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="51"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="52" t="s">
+      <c r="V7" s="43"/>
+      <c r="W7" s="35"/>
+    </row>
+    <row r="8" spans="1:23" ht="27.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="53"/>
-      <c r="J8" s="52" t="s">
+      <c r="I8" s="31"/>
+      <c r="J8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="53"/>
-      <c r="L8" s="54" t="s">
+      <c r="K8" s="31"/>
+      <c r="L8" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="54" t="s">
+      <c r="M8" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="51"/>
-      <c r="O8" s="52" t="s">
+      <c r="N8" s="25"/>
+      <c r="O8" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="52" t="s">
+      <c r="P8" s="31"/>
+      <c r="Q8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="R8" s="53"/>
-      <c r="S8" s="32" t="s">
+      <c r="R8" s="31"/>
+      <c r="S8" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="T8" s="34" t="s">
+      <c r="T8" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="U8" s="39"/>
-      <c r="V8" s="40"/>
-      <c r="W8" s="41"/>
-    </row>
-    <row r="9" spans="1:23" ht="15.6" thickTop="1" thickBot="1">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="29"/>
+    </row>
+    <row r="9" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1247,9 +1221,9 @@
       <c r="K9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="26"/>
       <c r="O9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1262,19 +1236,19 @@
       <c r="R9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S9" s="33"/>
-      <c r="T9" s="35"/>
-      <c r="U9" s="15" t="s">
+      <c r="S9" s="26"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="V9" s="15" t="s">
+      <c r="V9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="W9" s="15" t="s">
+      <c r="W9" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15.6" thickTop="1" thickBot="1">
+    <row r="10" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
@@ -1283,100 +1257,459 @@
       <c r="F10" s="6"/>
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="11"/>
+      <c r="I10" s="10"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="12"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="11"/>
       <c r="O10" s="9"/>
-      <c r="P10" s="11"/>
+      <c r="P10" s="10"/>
       <c r="Q10" s="9"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="17"/>
-      <c r="W10" s="18"/>
-    </row>
-    <row r="11" spans="1:23" ht="15.6" thickTop="1" thickBot="1">
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="15"/>
+    </row>
+    <row r="11" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="6"/>
       <c r="E11" s="8"/>
       <c r="F11" s="6"/>
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
-      <c r="I11" s="11"/>
+      <c r="I11" s="10"/>
       <c r="J11" s="9"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="12"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="11"/>
       <c r="O11" s="9"/>
-      <c r="P11" s="11"/>
+      <c r="P11" s="10"/>
       <c r="Q11" s="9"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="18"/>
-    </row>
-    <row r="12" spans="1:23" ht="15.6" thickTop="1" thickBot="1">
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="15"/>
+    </row>
+    <row r="12" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="C12" s="7"/>
       <c r="D12" s="6"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
       <c r="G12" s="8"/>
       <c r="H12" s="9"/>
-      <c r="I12" s="11"/>
+      <c r="I12" s="10"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="20"/>
-      <c r="W12" s="21"/>
-    </row>
-    <row r="13" spans="1:23" ht="15.6" thickTop="1" thickBot="1">
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="15"/>
+    </row>
+    <row r="13" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="7"/>
       <c r="D13" s="6"/>
       <c r="E13" s="8"/>
       <c r="F13" s="6"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="11"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="10"/>
       <c r="J13" s="9"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="11"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="10"/>
       <c r="Q13" s="9"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="22"/>
-      <c r="V13" s="20"/>
-      <c r="W13" s="21"/>
-    </row>
-    <row r="14" spans="1:23" ht="15" thickTop="1"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="15"/>
+    </row>
+    <row r="14" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="15"/>
+    </row>
+    <row r="15" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="15"/>
+    </row>
+    <row r="16" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="15"/>
+    </row>
+    <row r="17" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="15"/>
+    </row>
+    <row r="18" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="15"/>
+    </row>
+    <row r="19" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="15"/>
+    </row>
+    <row r="20" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="15"/>
+    </row>
+    <row r="21" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="14"/>
+      <c r="W21" s="15"/>
+    </row>
+    <row r="22" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="14"/>
+      <c r="W22" s="15"/>
+    </row>
+    <row r="23" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="14"/>
+      <c r="W23" s="15"/>
+    </row>
+    <row r="24" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="14"/>
+      <c r="W24" s="15"/>
+    </row>
+    <row r="25" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="14"/>
+      <c r="W25" s="15"/>
+    </row>
+    <row r="26" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="14"/>
+      <c r="W26" s="15"/>
+    </row>
+    <row r="27" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="14"/>
+      <c r="W27" s="15"/>
+    </row>
+    <row r="28" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="U7:W8"/>
+    <mergeCell ref="C2:W6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="O7:T7"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="H7:M7"/>
     <mergeCell ref="H8:I8"/>
@@ -1386,15 +1719,6 @@
     <mergeCell ref="D7:E8"/>
     <mergeCell ref="F7:G8"/>
     <mergeCell ref="C7:C9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="U7:W8"/>
-    <mergeCell ref="C2:W6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="N7:N9"/>
-    <mergeCell ref="O7:T7"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>